<commit_message>
Added a work log and updated time
</commit_message>
<xml_diff>
--- a/TimeTracking.xlsx
+++ b/TimeTracking.xlsx
@@ -8,23 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thomasbioren/Repositories/rhit-thesis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1199A858-3640-7642-8C2B-10BD21E13CA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B11311CE-36A3-D340-8804-F3DFF9A927C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{13DC4565-6128-064E-ABEB-12E1D5DAC89C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v2.0" hidden="1">Sheet1!$A$3:$A$13</definedName>
-    <definedName name="_xlchart.v2.1" hidden="1">Sheet1!$B$2</definedName>
-    <definedName name="_xlchart.v2.2" hidden="1">Sheet1!$B$3:$B$13</definedName>
-    <definedName name="_xlchart.v2.3" hidden="1">Sheet1!$C$2</definedName>
-    <definedName name="_xlchart.v2.4" hidden="1">Sheet1!$C$3:$C$13</definedName>
-    <definedName name="_xlchart.v2.5" hidden="1">Sheet1!$D$2</definedName>
-    <definedName name="_xlchart.v2.6" hidden="1">Sheet1!$D$3:$D$13</definedName>
-  </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -83,16 +74,16 @@
     <t>Week 11</t>
   </si>
   <si>
-    <t>Time Spent</t>
+    <t>Fall Quarter</t>
   </si>
   <si>
-    <t>Time Remaining</t>
+    <t>Ideal Time Worked</t>
   </si>
   <si>
-    <t>Ideal Time Remaining</t>
+    <t>Total Time Worked</t>
   </si>
   <si>
-    <t>Fall Quarter</t>
+    <t>Time Worked This Week</t>
   </si>
 </sst>
 </file>
@@ -207,7 +198,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Fall Quarter Burndown Chart</a:t>
+              <a:t>Fall Quarter Burnup Chart</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -256,7 +247,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Time Remaining</c:v>
+                  <c:v>Total Time Worked</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -300,7 +291,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="75000"/>
@@ -391,10 +382,10 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>129.5</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>#N/A</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>#N/A</c:v>
@@ -442,7 +433,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Ideal Time Remaining</c:v>
+                  <c:v>Ideal Time Worked</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -522,37 +513,37 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>84</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>108</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>120</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>108</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>96</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>84</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>72</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>60</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>48</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>36</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>12</c:v>
-                </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>120</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1671,21 +1662,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EFCD75A-D1E6-E74A-BD49-61DCE59EC750}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" zoomScale="109" workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.6640625" customWidth="1"/>
-    <col min="2" max="2" width="11.5" style="2" customWidth="1"/>
+    <col min="2" max="2" width="20.6640625" style="2" customWidth="1"/>
     <col min="3" max="3" width="16.83203125" style="2" customWidth="1"/>
     <col min="4" max="4" width="19.33203125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -1696,13 +1687,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>13</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -1710,28 +1701,30 @@
         <v>1</v>
       </c>
       <c r="B3" s="2">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="C3" s="2">
-        <f>IF(B3&gt;0,132-B3,#N/A)</f>
-        <v>129.5</v>
+        <f>IF(B3&gt;0,B3,#N/A)</f>
+        <v>3</v>
       </c>
       <c r="D3" s="2">
-        <f>132-12</f>
-        <v>120</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="2" t="e">
-        <f>IF(B4&gt;0,C3-B4,#N/A)</f>
-        <v>#N/A</v>
+      <c r="B4" s="2">
+        <v>1</v>
+      </c>
+      <c r="C4" s="2">
+        <f>IF(B4&gt;0,C3+B4,#N/A)</f>
+        <v>4</v>
       </c>
       <c r="D4" s="2">
-        <f>D3-12</f>
-        <v>108</v>
+        <f>D3+12</f>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -1739,12 +1732,12 @@
         <v>3</v>
       </c>
       <c r="C5" s="2" t="e">
-        <f t="shared" ref="C5:C13" si="0">IF(B5&gt;0,C4-B5,#N/A)</f>
+        <f t="shared" ref="C5:C13" si="0">IF(B5&gt;0,C4+B5,#N/A)</f>
         <v>#N/A</v>
       </c>
       <c r="D5" s="2">
-        <f t="shared" ref="D5:D13" si="1">D4-12</f>
-        <v>96</v>
+        <f t="shared" ref="D5:D13" si="1">D4+12</f>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -1757,7 +1750,7 @@
       </c>
       <c r="D6" s="2">
         <f t="shared" si="1"/>
-        <v>84</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -1770,7 +1763,7 @@
       </c>
       <c r="D7" s="2">
         <f t="shared" si="1"/>
-        <v>72</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -1783,7 +1776,7 @@
       </c>
       <c r="D8" s="2">
         <f t="shared" si="1"/>
-        <v>60</v>
+        <v>72</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -1796,7 +1789,7 @@
       </c>
       <c r="D9" s="2">
         <f t="shared" si="1"/>
-        <v>48</v>
+        <v>84</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -1809,7 +1802,7 @@
       </c>
       <c r="D10" s="2">
         <f t="shared" si="1"/>
-        <v>36</v>
+        <v>96</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -1822,7 +1815,7 @@
       </c>
       <c r="D11" s="2">
         <f t="shared" si="1"/>
-        <v>24</v>
+        <v>108</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -1835,7 +1828,7 @@
       </c>
       <c r="D12" s="2">
         <f t="shared" si="1"/>
-        <v>12</v>
+        <v>120</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -1847,8 +1840,7 @@
         <v>#N/A</v>
       </c>
       <c r="D13" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>120</v>
       </c>
     </row>
   </sheetData>

</xml_diff>